<commit_message>
Updated Sprint 2 product backlog
</commit_message>
<xml_diff>
--- a/Milestone 2/Product Backlog 2022.09.18.xlsx
+++ b/Milestone 2/Product Backlog 2022.09.18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Items\Education\Semester 6\COSC2299 - Software Eng Process &amp; Tools\Assignment 1\SEPT2022\Milestone 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EF8A4D-E2DB-4C7D-BC66-452C69B7C1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FEEEC-3D59-4A32-8FCD-502F9C7D7DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>As a patient, I want to view my payment history</t>
+  </si>
+  <si>
+    <t>DEFINITION OF DONE</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Code build without error, Code reviewed, Acceptance criteria met, Unit test passed, Functional test passed</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -469,6 +478,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -482,7 +500,37 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -777,13 +825,13 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.625" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="9" customWidth="1"/>
@@ -792,11 +840,11 @@
     <col min="5" max="5" width="11.125" style="30" customWidth="1"/>
     <col min="6" max="6" width="10.125" style="33" customWidth="1"/>
     <col min="7" max="7" width="20.125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="2" customWidth="1"/>
+    <col min="8" max="8" width="82.125" customWidth="1"/>
+    <col min="9" max="9" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
@@ -806,8 +854,10 @@
       <c r="E2" s="31"/>
       <c r="F2" s="34"/>
       <c r="G2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="14"/>
@@ -815,8 +865,10 @@
       <c r="E3" s="31"/>
       <c r="F3" s="34"/>
       <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="15" t="s">
         <v>1</v>
@@ -836,8 +888,14 @@
       <c r="G4" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="19">
         <v>1</v>
@@ -857,8 +915,12 @@
       <c r="G5" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H5" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="21">
         <v>2</v>
@@ -878,8 +940,12 @@
       <c r="G6" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="21">
         <v>3</v>
@@ -899,8 +965,12 @@
       <c r="G7" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="21">
         <v>4</v>
@@ -920,8 +990,12 @@
       <c r="G8" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="21">
         <v>5</v>
@@ -941,8 +1015,12 @@
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19">
         <v>6</v>
@@ -962,8 +1040,12 @@
       <c r="G10" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="H10" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="21">
         <v>7</v>
@@ -983,8 +1065,12 @@
       <c r="G11" s="29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="21">
         <v>8</v>
@@ -1004,8 +1090,12 @@
       <c r="G12" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="40"/>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="21">
         <v>9</v>
@@ -1025,8 +1115,12 @@
       <c r="G13" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="21">
         <v>10</v>
@@ -1046,8 +1140,12 @@
       <c r="G14" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="40"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19">
         <v>11</v>
@@ -1067,8 +1165,12 @@
       <c r="G15" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="40"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="21">
         <v>12</v>
@@ -1088,8 +1190,12 @@
       <c r="G16" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="40"/>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="21">
         <v>13</v>
@@ -1109,8 +1215,12 @@
       <c r="G17" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="21">
         <v>14</v>
@@ -1130,8 +1240,12 @@
       <c r="G18" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="21">
         <v>15</v>
@@ -1151,8 +1265,12 @@
       <c r="G19" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="21">
         <v>16</v>
@@ -1172,8 +1290,12 @@
       <c r="G20" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -1181,8 +1303,10 @@
       <c r="E21" s="28"/>
       <c r="F21" s="37"/>
       <c r="G21" s="28"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
@@ -1190,8 +1314,10 @@
       <c r="E22" s="28"/>
       <c r="F22" s="37"/>
       <c r="G22" s="28"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -1199,8 +1325,10 @@
       <c r="E23" s="28"/>
       <c r="F23" s="37"/>
       <c r="G23" s="28"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -1208,8 +1336,10 @@
       <c r="E24" s="28"/>
       <c r="F24" s="37"/>
       <c r="G24" s="28"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="19"/>
       <c r="C25" s="22"/>
@@ -1217,8 +1347,10 @@
       <c r="E25" s="28"/>
       <c r="F25" s="37"/>
       <c r="G25" s="28"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -1226,8 +1358,10 @@
       <c r="E26" s="28"/>
       <c r="F26" s="37"/>
       <c r="G26" s="28"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -1235,8 +1369,10 @@
       <c r="E27" s="28"/>
       <c r="F27" s="37"/>
       <c r="G27" s="28"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
@@ -1244,8 +1380,10 @@
       <c r="E28" s="28"/>
       <c r="F28" s="37"/>
       <c r="G28" s="28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
@@ -1253,8 +1391,10 @@
       <c r="E29" s="32"/>
       <c r="F29" s="38"/>
       <c r="G29" s="32"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="19"/>
       <c r="C30" s="22"/>
@@ -1262,8 +1402,10 @@
       <c r="E30" s="28"/>
       <c r="F30" s="37"/>
       <c r="G30" s="28"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
@@ -1271,8 +1413,10 @@
       <c r="E31" s="28"/>
       <c r="F31" s="37"/>
       <c r="G31" s="28"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
@@ -1280,8 +1424,10 @@
       <c r="E32" s="28"/>
       <c r="F32" s="37"/>
       <c r="G32" s="28"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
@@ -1289,8 +1435,10 @@
       <c r="E33" s="28"/>
       <c r="F33" s="37"/>
       <c r="G33" s="28"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="21"/>
       <c r="C34" s="22"/>
@@ -1298,8 +1446,10 @@
       <c r="E34" s="28"/>
       <c r="F34" s="37"/>
       <c r="G34" s="28"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="19"/>
       <c r="C35" s="22"/>
@@ -1307,8 +1457,10 @@
       <c r="E35" s="28"/>
       <c r="F35" s="37"/>
       <c r="G35" s="28"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
@@ -1316,8 +1468,10 @@
       <c r="E36" s="28"/>
       <c r="F36" s="37"/>
       <c r="G36" s="28"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
@@ -1325,8 +1479,10 @@
       <c r="E37" s="28"/>
       <c r="F37" s="37"/>
       <c r="G37" s="28"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
@@ -1334,8 +1490,10 @@
       <c r="E38" s="28"/>
       <c r="F38" s="37"/>
       <c r="G38" s="28"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="19"/>
       <c r="C39" s="22"/>
@@ -1343,8 +1501,10 @@
       <c r="E39" s="28"/>
       <c r="F39" s="37"/>
       <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="21"/>
       <c r="C40" s="22"/>
@@ -1352,8 +1512,10 @@
       <c r="E40" s="28"/>
       <c r="F40" s="37"/>
       <c r="G40" s="28"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+    </row>
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="21"/>
       <c r="C41" s="22"/>
@@ -1361,8 +1523,10 @@
       <c r="E41" s="28"/>
       <c r="F41" s="37"/>
       <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
@@ -1370,8 +1534,10 @@
       <c r="E42" s="28"/>
       <c r="F42" s="37"/>
       <c r="G42" s="28"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
@@ -1379,8 +1545,10 @@
       <c r="E43" s="28"/>
       <c r="F43" s="37"/>
       <c r="G43" s="28"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="19"/>
       <c r="C44" s="22"/>
@@ -1388,8 +1556,10 @@
       <c r="E44" s="28"/>
       <c r="F44" s="37"/>
       <c r="G44" s="28"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="23"/>
       <c r="C45" s="10"/>
@@ -1397,10 +1567,17 @@
       <c r="E45" s="31"/>
       <c r="F45" s="34"/>
       <c r="G45" s="31"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G44">
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="2" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:I44">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>